<commit_message>
ICPro final  beta 3
</commit_message>
<xml_diff>
--- a/misc/spikes.xlsx
+++ b/misc/spikes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>RY_Th230</t>
   </si>
@@ -325,6 +325,66 @@
   </si>
   <si>
     <t>RYb_Th230</t>
+  </si>
+  <si>
+    <t>ID_Th229</t>
+  </si>
+  <si>
+    <t>229-ZCO118</t>
+  </si>
+  <si>
+    <t>229-ZCxxxx</t>
+  </si>
+  <si>
+    <t>testspike</t>
+  </si>
+  <si>
+    <t>RY_Th229</t>
+  </si>
+  <si>
+    <t>RX_Th229</t>
+  </si>
+  <si>
+    <t>CY_Th229</t>
+  </si>
+  <si>
+    <t>ID_Th229</t>
+  </si>
+  <si>
+    <t>229-ZCO118</t>
+  </si>
+  <si>
+    <t>229-ZCxxxx</t>
+  </si>
+  <si>
+    <t>testspike</t>
+  </si>
+  <si>
+    <t>RY_Th229</t>
+  </si>
+  <si>
+    <t>RX_Th229</t>
+  </si>
+  <si>
+    <t>CY_Th229</t>
+  </si>
+  <si>
+    <t>ID_Th229</t>
+  </si>
+  <si>
+    <t>229-ZCO118</t>
+  </si>
+  <si>
+    <t>229-ZCxxxx</t>
+  </si>
+  <si>
+    <t>RY_Th229</t>
+  </si>
+  <si>
+    <t>RX_Th229</t>
+  </si>
+  <si>
+    <t>CY_Th229</t>
   </si>
 </sst>
 </file>
@@ -648,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -776,6 +836,9 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -821,7 +884,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
@@ -836,6 +899,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="true"/>
@@ -1207,21 +1273,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B2" s="0">
         <v>16115.688</v>
@@ -1235,7 +1301,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="B3" s="0">
         <v>65535</v>

</xml_diff>